<commit_message>
Added read functionality to validate creations
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\UiPath\CMPG-323-Project-4-29903599\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E043E8-3715-4B63-A14C-0751152507EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DF9B46-4F3C-4CA8-B522-22B62A22C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="900" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="4500" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -689,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -916,7 +916,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,10 +1166,10 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>0</v>
@@ -1183,10 +1183,10 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1200,10 +1200,10 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>0</v>
@@ -1217,10 +1217,10 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>0</v>
@@ -1234,10 +1234,10 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
@@ -1251,10 +1251,10 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>0</v>
@@ -1268,10 +1268,10 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
@@ -1285,10 +1285,10 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>0</v>
@@ -1302,10 +1302,10 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
@@ -1319,10 +1319,10 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
@@ -1336,10 +1336,10 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
@@ -1353,10 +1353,10 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>0</v>
@@ -1370,10 +1370,10 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
@@ -1387,10 +1387,10 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
@@ -1404,10 +1404,10 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
@@ -1421,10 +1421,10 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
@@ -1438,10 +1438,10 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
@@ -1455,10 +1455,10 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
@@ -1472,10 +1472,10 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
@@ -1489,10 +1489,10 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
@@ -1506,10 +1506,10 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
@@ -1523,10 +1523,10 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
@@ -1540,10 +1540,10 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>

</xml_diff>